<commit_message>
add info about JK
</commit_message>
<xml_diff>
--- a/diploma/data/ZHK_statistics.xlsx
+++ b/diploma/data/ZHK_statistics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rustaveli14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дом Соболева</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOKOLNIKI</t>
   </si>
 </sst>
 </file>
@@ -261,13 +267,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG11" activeCellId="0" sqref="AG11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG7" activeCellId="0" sqref="AG7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.85"/>
@@ -793,8 +799,217 @@
       <c r="AF5" s="0" t="n">
         <v>55.812115</v>
       </c>
-      <c r="AG5" s="7" t="n">
+      <c r="AG5" s="5" t="n">
         <v>37.597872</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <f aca="false">(J6+K6+L6)/B6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false">I6-J6</f>
+        <v>10</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">33 * 146</f>
+        <v>4818</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <f aca="false">U6/V6</f>
+        <v>3</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>55.764016</v>
+      </c>
+      <c r="AG6" s="7" t="n">
+        <v>37.652657</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>763</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>986</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <f aca="false">(J7+K7+L7)/B7</f>
+        <v>0.521625163826999</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">I7-J7</f>
+        <v>673</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>45984</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>60.3</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <f aca="false">U7/V7</f>
+        <v>5.33333333333333</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>55.782995</v>
+      </c>
+      <c r="AG7" s="7" t="n">
+        <v>37.690437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>